<commit_message>
main2.py is a work in progress 4
</commit_message>
<xml_diff>
--- a/Input_lecct copy.xlsx
+++ b/Input_lecct copy.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fer/PycharmProjects/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8078AD13-7F66-044F-9372-A6C185813C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC5E9AB-FB23-3049-87DF-C398A3B04B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{D0582A75-A442-7A41-B2A5-85D1C2251066}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26920" xr2:uid="{D0582A75-A442-7A41-B2A5-85D1C2251066}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vertex" sheetId="3" r:id="rId1"/>
-    <sheet name="Arcs" sheetId="1" r:id="rId2"/>
-    <sheet name="Commodities" sheetId="2" r:id="rId3"/>
+    <sheet name="Arcs" sheetId="1" r:id="rId1"/>
+    <sheet name="Commodities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -410,46 +409,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49858E9-287D-4940-B877-90D9247CA0E9}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C6B190-B7FB-004A-909C-CF6F86B57582}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -577,7 +536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5607BFC-FA57-3646-8893-93BA788B94F9}">
   <dimension ref="A1:D5"/>
   <sheetViews>

</xml_diff>